<commit_message>
changes with new version adding
</commit_message>
<xml_diff>
--- a/Interview-Qusetions-docs/Javascript-questionnaire.xlsx
+++ b/Interview-Qusetions-docs/Javascript-questionnaire.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\interview-preparation-kits\Interview-Qusetions-docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79C4CEE-DF11-4C32-A5C5-EBEC9EDC5172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Javascript" sheetId="1" r:id="rId1"/>
     <sheet name="Question" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Interview " sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="198">
   <si>
     <t>Ans</t>
   </si>
@@ -1436,12 +1442,50 @@
   <si>
     <t>Infinite Loop</t>
   </si>
+  <si>
+    <t>premitive and non premitive data in javascript</t>
+  </si>
+  <si>
+    <t>In JavaScript, data types can be categorized as primitive and non-primitive (also known as reference types). String, Number, Boolean, undefine, null, symbol.</t>
+  </si>
+  <si>
+    <t>Non-Primitive or Reference Data Types: Represents a collection of key-value pairs and complex entities. Object, Array, Function, Date Map, Set, RegExp, etc.</t>
+  </si>
+  <si>
+    <t>Q.</t>
+  </si>
+  <si>
+    <t>What is Prototype in Javascript?</t>
+  </si>
+  <si>
+    <t>In JavaScript, the prototype is an inherent mechanism that allows objects to inherit properties and methods from other objects. Every JavaScript object has a prototype, which is essentially a reference to another object. 
+Prototype Chain
+Object Prototypes
+Inheritance
+Prototype Property
+Constructor Functions</t>
+  </si>
+  <si>
+    <t>Ans.</t>
+  </si>
+  <si>
+    <t>What is VAR global scope?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any variable declared outside of a function is said to have Global Scope. </t>
+  </si>
+  <si>
+    <t>What is the difference between UseMemo and Usecallback?</t>
+  </si>
+  <si>
+    <t>To summarize, the main difference between useCallback and useMemo is the type of value they return. useCallback returns a memoized callback function, while useMemo returns a memoized value.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1597,8 +1641,21 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0F0F0F"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1623,8 +1680,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1632,11 +1695,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1695,54 +1773,88 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="0"/>
+    <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1780,7 +1892,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1814,6 +1926,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1848,9 +1961,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2023,21 +2137,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B210"/>
   <sheetViews>
-    <sheetView topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="B210" sqref="B210"/>
+    <sheetView tabSelected="1" topLeftCell="A209" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="254.5703125" style="11" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8">
         <v>1</v>
       </c>
@@ -2045,7 +2159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="141.75">
+    <row r="2" spans="1:2" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2053,7 +2167,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -2061,7 +2175,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="31.5">
+    <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
@@ -2069,7 +2183,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>3</v>
       </c>
@@ -2077,7 +2191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>0</v>
       </c>
@@ -2085,7 +2199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>4</v>
       </c>
@@ -2093,7 +2207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>0</v>
       </c>
@@ -2101,7 +2215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>5</v>
       </c>
@@ -2109,7 +2223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="31.5">
+    <row r="13" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>0</v>
       </c>
@@ -2117,12 +2231,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="252">
+    <row r="14" spans="1:2" ht="252" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>6</v>
       </c>
@@ -2130,7 +2244,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>0</v>
       </c>
@@ -2138,7 +2252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>7</v>
       </c>
@@ -2146,7 +2260,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="31.5">
+    <row r="20" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>0</v>
       </c>
@@ -2154,7 +2268,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>8</v>
       </c>
@@ -2162,7 +2276,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="31.5">
+    <row r="23" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>0</v>
       </c>
@@ -2170,7 +2284,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>9</v>
       </c>
@@ -2178,7 +2292,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>0</v>
       </c>
@@ -2186,7 +2300,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>10</v>
       </c>
@@ -2194,7 +2308,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>0</v>
       </c>
@@ -2202,12 +2316,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>11</v>
       </c>
@@ -2215,7 +2329,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>0</v>
       </c>
@@ -2223,12 +2337,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>12</v>
       </c>
@@ -2236,7 +2350,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>0</v>
       </c>
@@ -2244,7 +2358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>13</v>
       </c>
@@ -2252,7 +2366,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="31.5">
+    <row r="40" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>0</v>
       </c>
@@ -2260,7 +2374,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>14</v>
       </c>
@@ -2268,7 +2382,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>0</v>
       </c>
@@ -2276,7 +2390,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>15</v>
       </c>
@@ -2284,7 +2398,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>0</v>
       </c>
@@ -2292,12 +2406,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="346.5">
+    <row r="47" spans="1:2" ht="346.5" x14ac:dyDescent="0.25">
       <c r="B47" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>16</v>
       </c>
@@ -2305,7 +2419,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>0</v>
       </c>
@@ -2313,17 +2427,17 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>17</v>
       </c>
@@ -2331,7 +2445,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>0</v>
       </c>
@@ -2339,7 +2453,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>18</v>
       </c>
@@ -2347,7 +2461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>0</v>
       </c>
@@ -2355,12 +2469,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>19</v>
       </c>
@@ -2368,7 +2482,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>0</v>
       </c>
@@ -2376,7 +2490,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>20</v>
       </c>
@@ -2384,7 +2498,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="31.5">
+    <row r="65" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>0</v>
       </c>
@@ -2392,7 +2506,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>21</v>
       </c>
@@ -2400,7 +2514,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>0</v>
       </c>
@@ -2408,27 +2522,27 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="47.25">
+    <row r="71" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B71" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>22</v>
       </c>
@@ -2436,7 +2550,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>0</v>
       </c>
@@ -2444,7 +2558,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>23</v>
       </c>
@@ -2452,7 +2566,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>0</v>
       </c>
@@ -2460,22 +2574,22 @@
         <v>110</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B81" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B82" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B83" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>24</v>
       </c>
@@ -2483,7 +2597,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>0</v>
       </c>
@@ -2491,12 +2605,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>25</v>
       </c>
@@ -2504,7 +2618,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>0</v>
       </c>
@@ -2512,7 +2626,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="8">
         <v>26</v>
       </c>
@@ -2520,7 +2634,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
         <v>0</v>
       </c>
@@ -2528,7 +2642,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <v>27</v>
       </c>
@@ -2536,7 +2650,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
         <v>0</v>
       </c>
@@ -2544,27 +2658,27 @@
         <v>127</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B98" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B99" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B100" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="8">
         <v>28</v>
       </c>
@@ -2572,7 +2686,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
         <v>0</v>
       </c>
@@ -2580,7 +2694,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="8">
         <v>29</v>
       </c>
@@ -2588,7 +2702,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
         <v>0</v>
       </c>
@@ -2596,7 +2710,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="8">
         <v>30</v>
       </c>
@@ -2604,7 +2718,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
         <v>0</v>
       </c>
@@ -2612,7 +2726,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="8">
         <v>31</v>
       </c>
@@ -2620,7 +2734,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
         <v>0</v>
       </c>
@@ -2628,40 +2742,40 @@
         <v>131</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B113" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B114" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B115" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B116" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B117" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B118" s="13"/>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B119" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="8">
         <v>32</v>
       </c>
@@ -2669,7 +2783,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
         <v>0</v>
       </c>
@@ -2677,22 +2791,22 @@
         <v>136</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B123" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B124" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B125" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="8">
         <v>33</v>
       </c>
@@ -2700,7 +2814,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
         <v>0</v>
       </c>
@@ -2708,72 +2822,72 @@
         <v>132</v>
       </c>
     </row>
-    <row r="129" spans="2:2">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="130" spans="2:2">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="131" spans="2:2">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="132" spans="2:2">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="134" spans="2:2">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="135" spans="2:2">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="136" spans="2:2">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="138" spans="2:2">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="139" spans="2:2">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="140" spans="2:2">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="141" spans="2:2">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="142" spans="2:2">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="143" spans="2:2">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B143" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="8">
         <v>34</v>
       </c>
@@ -2781,7 +2895,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
         <v>0</v>
       </c>
@@ -2789,112 +2903,112 @@
         <v>74</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B147" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B149" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B150" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B151" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B153" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B155" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B157" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B158" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B160" s="11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="162" spans="2:2">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="163" spans="2:2">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="165" spans="2:2">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="166" spans="2:2">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="168" spans="2:2">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="169" spans="2:2">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="170" spans="2:2">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="2:2">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="173" spans="2:2">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="174" spans="2:2">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" s="11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="175" spans="2:2">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="176" spans="2:2">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="8">
         <v>35</v>
       </c>
@@ -2902,7 +3016,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="8" t="s">
         <v>0</v>
       </c>
@@ -2910,12 +3024,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B180" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="8">
         <v>36</v>
       </c>
@@ -2923,7 +3037,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="8" t="s">
         <v>0</v>
       </c>
@@ -2931,17 +3045,17 @@
         <v>97</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B184" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B185" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="8">
         <v>37</v>
       </c>
@@ -2949,7 +3063,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="8" t="s">
         <v>0</v>
       </c>
@@ -2957,7 +3071,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="8">
         <v>38</v>
       </c>
@@ -2965,7 +3079,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="8" t="s">
         <v>0</v>
       </c>
@@ -2973,59 +3087,59 @@
         <v>101</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B192" s="9"/>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B193" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B194" s="14"/>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B195" s="15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B196" s="16" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B197" s="17" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B198" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B199" s="18"/>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B200" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B201" s="19" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="8">
         <v>40</v>
       </c>
-      <c r="B203" s="32" t="s">
+      <c r="B203" s="22" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="30">
+    <row r="204" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="8" t="s">
         <v>0</v>
       </c>
@@ -3033,28 +3147,28 @@
         <v>143</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="8">
         <v>41</v>
       </c>
-      <c r="B206" s="32" t="s">
+      <c r="B206" s="22" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="8" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="8">
         <v>42</v>
       </c>
-      <c r="B209" s="32" t="s">
+      <c r="B209" s="22" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="315">
+    <row r="210" spans="1:2" ht="315" x14ac:dyDescent="0.25">
       <c r="A210" s="8" t="s">
         <v>148</v>
       </c>
@@ -3070,307 +3184,311 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="30"/>
-    <col min="2" max="2" width="173.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="23" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="9.140625" style="28"/>
+    <col min="2" max="2" width="173.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="30" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="30">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="28">
         <v>1</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="60">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="32" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="30">
+    <row r="3" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37">
         <v>2</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="38" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="30">
-      <c r="A4" s="30" t="s">
+      <c r="C3" s="39"/>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="33" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="B5" s="28"/>
-    </row>
-    <row r="6" spans="1:2" ht="30">
-      <c r="B6" s="29" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="34"/>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="33" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="30">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="28">
         <v>3</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="29" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="105">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="35" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="30">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="28">
         <v>4</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="29" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="30" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="36" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="30">
+    <row r="14" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="37">
         <v>5</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="38" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="390">
-      <c r="A15" s="30" t="s">
+      <c r="C14" s="39"/>
+    </row>
+    <row r="15" spans="1:3" ht="390" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="35" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="30">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="28">
         <v>6</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="29" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="45">
-      <c r="A18" s="30" t="s">
+    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="35" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="30">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="28">
         <v>7</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="29" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="30" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="35" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="30">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="28">
         <v>8</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="29" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="30" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="35" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="30">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="28">
         <v>9</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="29" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="30">
-      <c r="A27" s="30" t="s">
+    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="35" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="30">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="28">
         <v>10</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="29" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="30" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="B31" s="25" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="35" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="30">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="28">
         <v>11</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="29" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="30" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="28" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="30">
+    <row r="35" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="37">
         <v>12</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="43" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="30" t="s">
+      <c r="C35" s="39"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="35" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="30">
+    <row r="38" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="37">
         <v>13</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="43" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="30" t="s">
+      <c r="C38" s="39"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="35" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="30">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="28">
         <v>14</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="41" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="30" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="28" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="30">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="28">
         <v>15</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="41" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="30" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="B45" s="35" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="30">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="28">
         <v>16</v>
       </c>
-      <c r="B47" s="31" t="s">
+      <c r="B47" s="41" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="30" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="28" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="30">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="28">
         <v>17</v>
       </c>
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="41" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="16.5">
-      <c r="A51" s="30" t="s">
+    <row r="51" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A51" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="B51" s="34" t="s">
+      <c r="B51" s="42" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="30">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="28">
         <v>18</v>
       </c>
-      <c r="B53" s="31" t="s">
+      <c r="B53" s="41" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="30" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B54" s="24" t="s">
+      <c r="B54" s="35" t="s">
         <v>185</v>
       </c>
     </row>
@@ -3381,13 +3499,91 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="44"/>
+    <col min="2" max="2" width="140.85546875" style="25" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="126" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated with new js code
</commit_message>
<xml_diff>
--- a/Interview-Qusetions-docs/Javascript-questionnaire.xlsx
+++ b/Interview-Qusetions-docs/Javascript-questionnaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\interview-preparation-kits\Interview-Qusetions-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04073744-094E-40E5-8006-7F1CB040A3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182F74C6-17C6-40F3-B33A-6F1C9BFF2FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2131,8 +2131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2557,7 +2557,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>0</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
         <v>46</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>0</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B165" s="1" t="s">
         <v>86</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
         <v>0</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
added some changes of js and documentations
</commit_message>
<xml_diff>
--- a/Interview-Qusetions-docs/Javascript-questionnaire.xlsx
+++ b/Interview-Qusetions-docs/Javascript-questionnaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\interview-preparation-kits\Interview-Qusetions-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182F74C6-17C6-40F3-B33A-6F1C9BFF2FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1727B370-D120-41CE-90B3-845D4BF7F9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2131,8 +2131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2320,7 +2320,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>